<commit_message>
jn:dominios de variables para las bases existentes
</commit_message>
<xml_diff>
--- a/05_Entregable 3/previo/Diccionarios/MD_01_Fiscalía_Informe_estadistico_2025012322001116 FIscalia.xlsx
+++ b/05_Entregable 3/previo/Diccionarios/MD_01_Fiscalía_Informe_estadistico_2025012322001116 FIscalia.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Javi_Angelito\wcs\04_Entregable 2\envio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Javi_Angelito\wcs\05_Entregable 3\previo\Diccionarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0860176-6EB8-4985-8BB2-4E021C54FAC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F6A610-1AED-458F-BE08-72205285C5A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadatos generales" sheetId="1" r:id="rId1"/>
-    <sheet name="02_1_general" sheetId="4" r:id="rId2"/>
-    <sheet name="02_1_diccionario" sheetId="3" r:id="rId3"/>
+    <sheet name="01_1_general" sheetId="4" r:id="rId2"/>
+    <sheet name="01_1_diccionario" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="91">
   <si>
     <t>Elemento</t>
   </si>
@@ -62,18 +62,12 @@
     <t>1.0</t>
   </si>
   <si>
-    <t>Nombre de la variable</t>
-  </si>
-  <si>
     <t>Definición</t>
   </si>
   <si>
     <t>Formato de Datos</t>
   </si>
   <si>
-    <t>Unidad de Medida</t>
-  </si>
-  <si>
     <t>Fuente de Datos</t>
   </si>
   <si>
@@ -300,6 +294,12 @@
   </si>
   <si>
     <t>Definir/depurar las categorías de la variable</t>
+  </si>
+  <si>
+    <t>Nombre actual</t>
+  </si>
+  <si>
+    <t>Nombre propuesto</t>
   </si>
 </sst>
 </file>
@@ -771,67 +771,67 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C7" s="8"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -846,15 +846,15 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="B6" sqref="B6"/>
-      <selection pane="topRight" activeCell="G1" activeCellId="1" sqref="F1:F1048576 G1:G1048576"/>
+      <selection pane="topRight" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1"/>
+    <col min="3" max="3" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
@@ -863,45 +863,46 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>56</v>
+        <v>36</v>
+      </c>
+      <c r="B2" s="11" t="str">
+        <f>LOWER(A2)</f>
+        <v>fecha_registro</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>6</v>
@@ -912,43 +913,45 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>58</v>
+        <v>37</v>
+      </c>
+      <c r="B3" s="11" t="str">
+        <f t="shared" ref="B3:B18" si="0">LOWER(A3)</f>
+        <v>d_ndd</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H3" s="11"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>62</v>
+        <v>38</v>
+      </c>
+      <c r="B4" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>d_anio_registro</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>6</v>
@@ -960,19 +963,20 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>59</v>
+        <v>39</v>
+      </c>
+      <c r="B5" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>d_fecha_incidente</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>6</v>
@@ -984,19 +988,20 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>63</v>
+        <v>40</v>
+      </c>
+      <c r="B6" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>d_mes_registro</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>6</v>
@@ -1008,19 +1013,20 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>60</v>
+        <v>41</v>
+      </c>
+      <c r="B7" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>d_mes_incidente</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>6</v>
@@ -1032,19 +1038,20 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>64</v>
+        <v>42</v>
+      </c>
+      <c r="B8" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>d_articulo</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>6</v>
@@ -1053,263 +1060,273 @@
         <v>247</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>65</v>
+        <v>43</v>
+      </c>
+      <c r="B9" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>d_delito</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>66</v>
+        <v>44</v>
+      </c>
+      <c r="B10" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>d_delito_circunstancial</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>6</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>67</v>
+        <v>45</v>
+      </c>
+      <c r="B11" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>d_estado_procesal</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F11" s="11" t="s">
         <v>6</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>68</v>
+        <v>46</v>
+      </c>
+      <c r="B12" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>d_etapa_actual</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F12" s="11" t="s">
         <v>6</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>61</v>
+        <v>47</v>
+      </c>
+      <c r="B13" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>d_provincia_incidente</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H13" s="11"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>69</v>
+        <v>48</v>
+      </c>
+      <c r="B14" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>d_canton_incidente</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H14" s="11"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>70</v>
+        <v>49</v>
+      </c>
+      <c r="B15" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>d_tipo_delito</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F15" s="11" t="s">
         <v>6</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>71</v>
+        <v>50</v>
+      </c>
+      <c r="B16" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>d_tipo_flagrante</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>6</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>d_estado_ndd</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>74</v>
-      </c>
       <c r="F17" s="11" t="s">
         <v>6</v>
       </c>
       <c r="G17" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="H17" s="11" t="s">
         <v>88</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>f_grupo_horainc</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="H18" s="11" t="s">
         <v>73</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
jn: informe producto 3 preliminar
</commit_message>
<xml_diff>
--- a/05_Entregable 3/previo/Diccionarios/MD_01_Fiscalía_Informe_estadistico_2025012322001116 FIscalia.xlsx
+++ b/05_Entregable 3/previo/Diccionarios/MD_01_Fiscalía_Informe_estadistico_2025012322001116 FIscalia.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Javi_Angelito\wcs\05_Entregable 3\previo\Diccionarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Disco_F\!!Personal\Mio\1_WCS 2024\wcs\05_Entregable 3\previo\Diccionarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F6A610-1AED-458F-BE08-72205285C5A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Metadatos generales" sheetId="1" r:id="rId1"/>
     <sheet name="01_1_general" sheetId="4" r:id="rId2"/>
     <sheet name="01_1_diccionario" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="108">
   <si>
     <t>Elemento</t>
   </si>
@@ -242,9 +241,6 @@
     <t>Estado de la noticia del delito</t>
   </si>
   <si>
-    <t>Granja horaria del incidente</t>
-  </si>
-  <si>
     <t>Clasificación interna Fiscalía</t>
   </si>
   <si>
@@ -300,12 +296,66 @@
   </si>
   <si>
     <t>Nombre propuesto</t>
+  </si>
+  <si>
+    <t>fecha_registro</t>
+  </si>
+  <si>
+    <t>ndd</t>
+  </si>
+  <si>
+    <t>anio_registro</t>
+  </si>
+  <si>
+    <t>fecha_incidente</t>
+  </si>
+  <si>
+    <t>mes_registro</t>
+  </si>
+  <si>
+    <t>mes_incidente</t>
+  </si>
+  <si>
+    <t>articulo</t>
+  </si>
+  <si>
+    <t>delito</t>
+  </si>
+  <si>
+    <t>delito_circunstancial</t>
+  </si>
+  <si>
+    <t>estado_procesal</t>
+  </si>
+  <si>
+    <t>etapa_actual</t>
+  </si>
+  <si>
+    <t>provincia_incidente</t>
+  </si>
+  <si>
+    <t>canton_incidente</t>
+  </si>
+  <si>
+    <t>tipo_delito</t>
+  </si>
+  <si>
+    <t>tipo_flagrante</t>
+  </si>
+  <si>
+    <t>estado_ndd</t>
+  </si>
+  <si>
+    <t>grupo_horainc</t>
+  </si>
+  <si>
+    <t>Franja horaria del incidente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -382,7 +432,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -409,6 +459,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -688,7 +739,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -756,7 +807,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -840,13 +891,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="B6" sqref="B6"/>
-      <selection pane="topRight" activeCell="B23" sqref="B23"/>
+      <selection pane="topRight" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,10 +914,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>89</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>11</v>
@@ -891,9 +942,8 @@
       <c r="A2" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="11" t="str">
-        <f>LOWER(A2)</f>
-        <v>fecha_registro</v>
+      <c r="B2" s="11" t="s">
+        <v>90</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>54</v>
@@ -915,9 +965,8 @@
       <c r="A3" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="11" t="str">
-        <f t="shared" ref="B3:B18" si="0">LOWER(A3)</f>
-        <v>d_ndd</v>
+      <c r="B3" s="11" t="s">
+        <v>91</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>56</v>
@@ -932,7 +981,7 @@
         <v>29</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H3" s="11"/>
     </row>
@@ -940,9 +989,8 @@
       <c r="A4" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>d_anio_registro</v>
+      <c r="B4" s="11" t="s">
+        <v>92</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>60</v>
@@ -951,7 +999,7 @@
         <v>27</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>6</v>
@@ -965,9 +1013,8 @@
       <c r="A5" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>d_fecha_incidente</v>
+      <c r="B5" s="11" t="s">
+        <v>93</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>57</v>
@@ -990,9 +1037,8 @@
       <c r="A6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>d_mes_registro</v>
+      <c r="B6" s="11" t="s">
+        <v>94</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>61</v>
@@ -1001,7 +1047,7 @@
         <v>27</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>6</v>
@@ -1015,9 +1061,8 @@
       <c r="A7" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>d_mes_incidente</v>
+      <c r="B7" s="11" t="s">
+        <v>95</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>58</v>
@@ -1026,7 +1071,7 @@
         <v>27</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>6</v>
@@ -1037,12 +1082,11 @@
       <c r="H7" s="11"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>d_articulo</v>
+      <c r="B8" s="11" t="s">
+        <v>96</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>62</v>
@@ -1051,7 +1095,7 @@
         <v>27</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>6</v>
@@ -1060,16 +1104,15 @@
         <v>247</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>d_delito</v>
+      <c r="B9" s="11" t="s">
+        <v>97</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>63</v>
@@ -1078,25 +1121,24 @@
         <v>27</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>d_delito_circunstancial</v>
+      <c r="B10" s="11" t="s">
+        <v>98</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>64</v>
@@ -1105,25 +1147,24 @@
         <v>27</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>6</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>d_estado_procesal</v>
+      <c r="B11" s="11" t="s">
+        <v>99</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>65</v>
@@ -1132,25 +1173,24 @@
         <v>27</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F11" s="11" t="s">
         <v>6</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>d_etapa_actual</v>
+      <c r="B12" s="11" t="s">
+        <v>100</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>66</v>
@@ -1159,25 +1199,24 @@
         <v>27</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F12" s="11" t="s">
         <v>6</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>d_provincia_incidente</v>
+      <c r="B13" s="11" t="s">
+        <v>101</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>59</v>
@@ -1186,13 +1225,13 @@
         <v>27</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H13" s="11"/>
     </row>
@@ -1200,9 +1239,8 @@
       <c r="A14" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>d_canton_incidente</v>
+      <c r="B14" s="11" t="s">
+        <v>102</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>67</v>
@@ -1211,23 +1249,22 @@
         <v>27</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H14" s="11"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>d_tipo_delito</v>
+      <c r="B15" s="11" t="s">
+        <v>103</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>68</v>
@@ -1236,25 +1273,24 @@
         <v>27</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F15" s="11" t="s">
         <v>6</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>d_tipo_flagrante</v>
+      <c r="B16" s="11" t="s">
+        <v>104</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>69</v>
@@ -1263,25 +1299,24 @@
         <v>27</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>6</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>d_estado_ndd</v>
+      <c r="B17" s="11" t="s">
+        <v>105</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>70</v>
@@ -1290,43 +1325,42 @@
         <v>27</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F17" s="11" t="s">
         <v>6</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>f_grupo_horainc</v>
+      <c r="B18" s="11" t="s">
+        <v>106</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>71</v>
+        <v>107</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>27</v>
       </c>
       <c r="E18" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="H18" s="11" t="s">
         <v>72</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1334,10 +1368,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="G16:G18" xr:uid="{BF30A2B3-A246-49BE-8BFD-71ECCD1E58AB}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="G16:G18">
       <formula1>-1</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="G5:G6" xr:uid="{657C3B75-ABBA-428A-87F2-F4A97104B238}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="G5:G6">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
jn: informe producto 3 preliminar para revision ag
</commit_message>
<xml_diff>
--- a/05_Entregable 3/previo/Diccionarios/MD_01_Fiscalía_Informe_estadistico_2025012322001116 FIscalia.xlsx
+++ b/05_Entregable 3/previo/Diccionarios/MD_01_Fiscalía_Informe_estadistico_2025012322001116 FIscalia.xlsx
@@ -58,9 +58,6 @@
     <t>Diccionario de variables sobre tráfico de vida silvestre</t>
   </si>
   <si>
-    <t>1.0</t>
-  </si>
-  <si>
     <t>Definición</t>
   </si>
   <si>
@@ -350,6 +347,9 @@
   </si>
   <si>
     <t>Franja horaria del incidente</t>
+  </si>
+  <si>
+    <t>2.0</t>
   </si>
 </sst>
 </file>
@@ -743,7 +743,7 @@
   <dimension ref="A2:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,7 +773,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -822,67 +822,67 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" s="8"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -895,7 +895,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection activeCell="B6" sqref="B6"/>
       <selection pane="topRight" activeCell="B17" sqref="B17"/>
     </sheetView>
@@ -914,45 +914,45 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>89</v>
-      </c>
       <c r="C1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>6</v>
@@ -963,43 +963,43 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D3" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>29</v>
-      </c>
       <c r="G3" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H3" s="11"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>6</v>
@@ -1011,19 +1011,19 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>6</v>
@@ -1035,19 +1035,19 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>6</v>
@@ -1059,19 +1059,19 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>6</v>
@@ -1083,19 +1083,19 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>6</v>
@@ -1104,263 +1104,263 @@
         <v>247</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>6</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F11" s="11" t="s">
         <v>6</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F12" s="11" t="s">
         <v>6</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H13" s="11"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H14" s="11"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F15" s="11" t="s">
         <v>6</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>6</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C17" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>71</v>
-      </c>
       <c r="F17" s="11" t="s">
         <v>6</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B18" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="C18" s="11" t="s">
-        <v>107</v>
-      </c>
       <c r="D18" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E18" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="H18" s="11" t="s">
         <v>71</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>